<commit_message>
Afegida conductivitat del coure
</commit_message>
<xml_diff>
--- a/Treball/Altres/Adiabatic-flame-temperature-calculation.xlsx
+++ b/Treball/Altres/Adiabatic-flame-temperature-calculation.xlsx
@@ -1726,17 +1726,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="0"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="0.00E+00"/>
-    <numFmt numFmtId="171" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="General"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="171" formatCode="0.00E+00"/>
+    <numFmt numFmtId="172" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1848,6 +1849,16 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="0"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1858,7 +1869,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria Math"/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1874,6 +1885,11 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Cambria Math"/>
+      <family val="0"/>
+    </font>
+    <font>
       <i val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1884,7 +1900,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Symbol"/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1991,7 +2007,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="51">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2036,7 +2052,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2060,7 +2076,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2068,23 +2084,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2092,7 +2104,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2108,11 +2120,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2120,15 +2128,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2136,7 +2144,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2152,11 +2160,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2168,20 +2172,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2208,7 +2204,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2300,9 +2296,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>93600</xdr:colOff>
+      <xdr:colOff>93240</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:rowOff>53640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2311,18 +2307,18 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8004240" y="7309800"/>
-          <a:ext cx="4630320" cy="8055720"/>
+          <a:off x="8002800" y="7309800"/>
+          <a:ext cx="4631040" cy="8000640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="bg1"/>
+          <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="19080">
           <a:solidFill>
-            <a:schemeClr val="tx1"/>
+            <a:srgbClr val="ffffff"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
@@ -2344,7 +2340,7 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -2354,7 +2350,7 @@
           </a:r>
           <a:br/>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -2373,7 +2369,7 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -2383,7 +2379,7 @@
           </a:r>
           <a:br/>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -2412,7 +2408,7 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike" u="sng">
+            <a:rPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike" u="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -2422,7 +2418,7 @@
             <a:t>Methane oxidation</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -2431,7 +2427,7 @@
             <a:t>:       </a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -2693,7 +2689,7 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3333,7 +3329,7 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3351,7 +3347,7 @@
             <a:t>〖𝐶</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3369,7 +3365,7 @@
             <a:t>〗</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3387,7 +3383,7 @@
             <a:t>〖𝐶</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3405,7 +3401,7 @@
             <a:t>〗</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3471,7 +3467,7 @@
             <a:t>T is the adiabatic flame temperature </a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3627,9 +3623,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>671760</xdr:colOff>
+      <xdr:colOff>671400</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>49680</xdr:rowOff>
+      <xdr:rowOff>49320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3642,8 +3638,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4110840" y="1035720"/>
-          <a:ext cx="3529800" cy="1461600"/>
+          <a:off x="4109760" y="1035720"/>
+          <a:ext cx="3529440" cy="1461240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3664,9 +3660,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>584280</xdr:colOff>
+      <xdr:colOff>583920</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3675,20 +3671,18 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14103720" y="8024760"/>
-          <a:ext cx="4692240" cy="2623680"/>
+          <a:off x="14103000" y="8024760"/>
+          <a:ext cx="4691880" cy="2623320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
+            <a:srgbClr val="ffffff"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
@@ -3885,182 +3879,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>38160</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>9360</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>600120</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>-47880</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp>
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name="Scroll Bar 2" descr="" hidden="0"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr anchor="ctr">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:p>
-              <a:r>
-                <a:t/>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>28440</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>218880</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>552240</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>218880</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp>
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name="Scroll Bar 3" descr="" hidden="0"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr anchor="ctr">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:p>
-              <a:r>
-                <a:t/>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>19080</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>209520</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>647640</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>200160</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp>
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name="Scroll Bar 4" descr="" hidden="0"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr anchor="ctr">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:p>
-              <a:r>
-                <a:t/>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>57240</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>19080</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>695160</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>-28440</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp>
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name="Scroll Bar 9" descr="" hidden="0"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr anchor="ctr">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:p>
-              <a:r>
-                <a:t/>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -4075,9 +3893,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>390240</xdr:colOff>
+      <xdr:colOff>389880</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>84960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4087,19 +3905,17 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="219240" y="2705040"/>
-          <a:ext cx="8619480" cy="2476080"/>
+          <a:ext cx="8623440" cy="2475720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
+            <a:srgbClr val="ffffff"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
@@ -4214,7 +4030,7 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4232,7 +4048,7 @@
             <a:t>〖𝐶</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4250,7 +4066,7 @@
             <a:t>〗</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4268,7 +4084,7 @@
             <a:t>〖</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4286,7 +4102,7 @@
             <a:t>〗</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4304,7 +4120,7 @@
             <a:t>〖</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4322,7 +4138,7 @@
             <a:t>〗</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4340,7 +4156,7 @@
             <a:t>〖</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4358,7 +4174,7 @@
             <a:t>〗</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4387,7 +4203,7 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4406,7 +4222,7 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4433,7 +4249,7 @@
             <a:t>Δ</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4451,7 +4267,7 @@
             <a:t>〗</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4469,7 +4285,7 @@
             <a:t>〖𝐶</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4487,22 +4303,13 @@
             <a:t>〗</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" sz="1100" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>)</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>= 0 = sum of cells C4 and K12</a:t>
+            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>)= 0 = sum of cells C4 and K12</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="ca-ES" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -4559,50 +4366,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>238320</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>114480</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>196920</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>105120</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp>
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name="Scroll Bar 1" descr="" hidden="0"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr anchor="ctr">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:p>
-              <a:r>
-                <a:t/>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -4613,15 +4376,15 @@
   </sheetPr>
   <dimension ref="A1:Z45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N28" activeCellId="0" sqref="N28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.28"/>
@@ -4696,9 +4459,12 @@
         <v>10</v>
       </c>
       <c r="B7" s="10" t="n">
-        <v>4891.4</v>
-      </c>
-      <c r="C7" s="11"/>
+        <v>3000</v>
+      </c>
+      <c r="C7" s="11" t="n">
+        <f aca="false">B7/1000</f>
+        <v>3</v>
+      </c>
       <c r="D7" s="11"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -4778,15 +4544,15 @@
       <c r="Q8" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="R8" s="22" t="n">
+      <c r="R8" s="16" t="n">
         <f aca="false">J8 + K8*Ti/1000 + L8*(Ti/1000)^2 + M8*(Ti/1000)^3 + N8/((Ti/1000)^2)</f>
         <v>71.794054</v>
       </c>
-      <c r="S8" s="23" t="n">
+      <c r="S8" s="22" t="n">
         <f aca="false">R8/1000</f>
         <v>0.071794054</v>
       </c>
-      <c r="Z8" s="24" t="n">
+      <c r="Z8" s="23" t="n">
         <f aca="false">'n-butane example problem'!G4+'n-butane example problem'!H4*TK+'n-butane example problem'!I4*TK^2+'n-butane example problem'!J4*TK^3</f>
         <v>48.7002</v>
       </c>
@@ -4824,21 +4590,21 @@
       <c r="O9" s="20" t="n">
         <v>-8.903471</v>
       </c>
-      <c r="P9" s="25" t="n">
+      <c r="P9" s="24" t="n">
         <v>0</v>
       </c>
       <c r="Q9" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="R9" s="22" t="n">
+      <c r="R9" s="16" t="n">
         <f aca="false">J9 + K9*Ti/1000 + L9*(Ti/1000)^2 + M9*(Ti/1000)^3 + N9/((Ti/1000)^2)</f>
         <v>32.439526</v>
       </c>
-      <c r="S9" s="23" t="n">
+      <c r="S9" s="22" t="n">
         <f aca="false">R9/1000</f>
         <v>0.032439526</v>
       </c>
-      <c r="Z9" s="24" t="n">
+      <c r="Z9" s="23" t="n">
         <f aca="false">'n-butane example problem'!G5+'n-butane example problem'!H5*TK+'n-butane example problem'!I5*TK^2+'n-butane example problem'!J5*TK^3</f>
         <v>37.281752</v>
       </c>
@@ -4876,21 +4642,21 @@
       <c r="O10" s="18" t="n">
         <v>-11.32468</v>
       </c>
-      <c r="P10" s="25" t="n">
+      <c r="P10" s="24" t="n">
         <v>0</v>
       </c>
       <c r="Q10" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="R10" s="22" t="n">
+      <c r="R10" s="16" t="n">
         <f aca="false">J10 + K10*Ti/1000 + L10*(Ti/1000)^2 + M10*(Ti/1000)^3 + N10/((Ti/1000)^2)</f>
         <v>34.863553</v>
       </c>
-      <c r="S10" s="23" t="n">
+      <c r="S10" s="22" t="n">
         <f aca="false">R10/1000</f>
         <v>0.034863553</v>
       </c>
-      <c r="Z10" s="24" t="n">
+      <c r="Z10" s="23" t="n">
         <f aca="false">'n-butane example problem'!G6+'n-butane example problem'!H6*TK+'n-butane example problem'!I6*TK^2+'n-butane example problem'!J6*TK^3</f>
         <v>35.492528</v>
       </c>
@@ -4923,21 +4689,21 @@
       <c r="O11" s="20" t="n">
         <v>5.337651</v>
       </c>
-      <c r="P11" s="25" t="n">
+      <c r="P11" s="24" t="n">
         <v>0</v>
       </c>
       <c r="Q11" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="R11" s="22" t="n">
+      <c r="R11" s="16" t="n">
         <f aca="false">J11 + K11*Ti/1000 + L11*(Ti/1000)^2 + M11*(Ti/1000)^3 + N11/((Ti/1000)^2)</f>
         <v>39.003383</v>
       </c>
-      <c r="S11" s="23" t="n">
+      <c r="S11" s="22" t="n">
         <f aca="false">R11/1000</f>
         <v>0.039003383</v>
       </c>
-      <c r="Z11" s="24" t="n">
+      <c r="Z11" s="23" t="n">
         <f aca="false">'n-butane example problem'!G7+'n-butane example problem'!H7*TK+'n-butane example problem'!I7*TK^2+'n-butane example problem'!J7*TK^3</f>
         <v>59.991448</v>
       </c>
@@ -4970,23 +4736,23 @@
       <c r="O12" s="20" t="n">
         <v>-8.671914</v>
       </c>
-      <c r="P12" s="25" t="n">
+      <c r="P12" s="24" t="n">
         <v>0</v>
       </c>
       <c r="Q12" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="R12" s="22" t="n">
+      <c r="R12" s="16" t="n">
         <f aca="false">J12 + K12*Ti/1000 + L12*(Ti/1000)^2 + M12*(Ti/1000)^3 + N12/((Ti/1000)^2)</f>
         <v>37.827617</v>
       </c>
-      <c r="S12" s="23" t="n">
+      <c r="S12" s="22" t="n">
         <f aca="false">R12/1000</f>
         <v>0.037827617</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="26"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="8"/>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
@@ -5013,23 +4779,23 @@
       <c r="O13" s="20" t="n">
         <v>-4.935202</v>
       </c>
-      <c r="P13" s="25" t="n">
+      <c r="P13" s="24" t="n">
         <v>0</v>
       </c>
       <c r="Q13" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="R13" s="22" t="n">
+      <c r="R13" s="16" t="n">
         <f aca="false">J13 + K13*Ti/1000 + L13*(Ti/1000)^2 + M13*(Ti/1000)^3 + N13/((Ti/1000)^2)</f>
         <v>32.6919</v>
       </c>
-      <c r="S13" s="23" t="n">
+      <c r="S13" s="22" t="n">
         <f aca="false">R13/1000</f>
         <v>0.0326919</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="26"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="8"/>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
@@ -5056,23 +4822,23 @@
       <c r="O14" s="18" t="n">
         <v>-18.97091</v>
       </c>
-      <c r="P14" s="25" t="n">
+      <c r="P14" s="24" t="n">
         <v>0</v>
       </c>
       <c r="Q14" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="R14" s="22" t="n">
+      <c r="R14" s="16" t="n">
         <f aca="false">J14 + K14*Ti/1000 + L14*(Ti/1000)^2 + M14*(Ti/1000)^3 + N14/((Ti/1000)^2)</f>
         <v>31.91216</v>
       </c>
-      <c r="S14" s="23" t="n">
+      <c r="S14" s="22" t="n">
         <f aca="false">R14/1000</f>
         <v>0.03191216</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="26" t="s">
         <v>34</v>
       </c>
       <c r="E15" s="17"/>
@@ -5106,17 +4872,17 @@
       <c r="Q15" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="R15" s="22" t="n">
+      <c r="R15" s="16" t="n">
         <f aca="false">J15 + K15*Ti/1000 + L15*(Ti/1000)^2 + M15*(Ti/1000)^3 + N15/((Ti/1000)^2)</f>
         <v>54.304762</v>
       </c>
-      <c r="S15" s="23" t="n">
+      <c r="S15" s="22" t="n">
         <f aca="false">R15/1000</f>
         <v>0.054304762</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="27" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="13" t="s">
@@ -5156,11 +4922,11 @@
       <c r="Q16" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="R16" s="22" t="n">
+      <c r="R16" s="16" t="n">
         <f aca="false">J16 + K16*Ti/1000 + L16*(Ti/1000)^2 + M16*(Ti/1000)^3 + N16/((Ti/1000)^2)</f>
         <v>53.985257</v>
       </c>
-      <c r="S16" s="23" t="n">
+      <c r="S16" s="22" t="n">
         <f aca="false">R16/1000</f>
         <v>0.053985257</v>
       </c>
@@ -5185,7 +4951,7 @@
       <c r="I17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="22" t="n">
+      <c r="J17" s="16" t="n">
         <v>30.092</v>
       </c>
       <c r="K17" s="21" t="n">
@@ -5200,20 +4966,20 @@
       <c r="N17" s="21" t="n">
         <v>0.082139</v>
       </c>
-      <c r="O17" s="29" t="n">
+      <c r="O17" s="28" t="n">
         <v>-250.881</v>
       </c>
-      <c r="P17" s="29" t="n">
+      <c r="P17" s="28" t="n">
         <v>-241.8264</v>
       </c>
       <c r="Q17" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="R17" s="22" t="n">
+      <c r="R17" s="16" t="n">
         <f aca="false">J17 + K17*Ti/1000 + L17*(Ti/1000)^2 + M17*(Ti/1000)^3 + N17/((Ti/1000)^2)</f>
         <v>41.265559</v>
       </c>
-      <c r="S17" s="23" t="n">
+      <c r="S17" s="22" t="n">
         <f aca="false">R17/1000</f>
         <v>0.041265559</v>
       </c>
@@ -5226,7 +4992,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="8" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D18" s="8" t="n">
         <v>0</v>
@@ -5238,7 +5004,7 @@
       <c r="I18" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J18" s="22" t="n">
+      <c r="J18" s="16" t="n">
         <v>41.964</v>
       </c>
       <c r="K18" s="21" t="n">
@@ -5250,23 +5016,23 @@
       <c r="M18" s="21" t="n">
         <v>0.09812</v>
       </c>
-      <c r="N18" s="22" t="n">
+      <c r="N18" s="16" t="n">
         <v>-11.15764</v>
       </c>
-      <c r="O18" s="29" t="n">
+      <c r="O18" s="28" t="n">
         <v>-272.1797</v>
       </c>
-      <c r="P18" s="29" t="n">
+      <c r="P18" s="28" t="n">
         <v>-241.8264</v>
       </c>
-      <c r="Q18" s="30" t="s">
+      <c r="Q18" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="R18" s="22" t="n">
+      <c r="R18" s="16" t="n">
         <f aca="false">J18 + K18*Ti/1000 + L18*(Ti/1000)^2 + M18*(Ti/1000)^3 + N18/((Ti/1000)^2)</f>
         <v>38.02668</v>
       </c>
-      <c r="S18" s="23" t="n">
+      <c r="S18" s="22" t="n">
         <f aca="false">R18/1000</f>
         <v>0.03802668</v>
       </c>
@@ -5293,35 +5059,35 @@
       <c r="I19" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="J19" s="31" t="n">
+      <c r="J19" s="29" t="n">
         <v>33.066178</v>
       </c>
-      <c r="K19" s="31" t="n">
+      <c r="K19" s="29" t="n">
         <v>-11.363417</v>
       </c>
-      <c r="L19" s="31" t="n">
+      <c r="L19" s="29" t="n">
         <v>11.432816</v>
       </c>
-      <c r="M19" s="31" t="n">
+      <c r="M19" s="29" t="n">
         <v>-2.772874</v>
       </c>
-      <c r="N19" s="31" t="n">
+      <c r="N19" s="29" t="n">
         <v>-0.158558</v>
       </c>
-      <c r="O19" s="31" t="n">
+      <c r="O19" s="29" t="n">
         <v>-9.980797</v>
       </c>
-      <c r="P19" s="31" t="n">
+      <c r="P19" s="29" t="n">
         <v>0</v>
       </c>
       <c r="Q19" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="R19" s="22" t="n">
+      <c r="R19" s="16" t="n">
         <f aca="false">J19 + K19*Ti/1000 + L19*(Ti/1000)^2 + M19*(Ti/1000)^3 + N19/((Ti/1000)^2)</f>
         <v>30.204145</v>
       </c>
-      <c r="S19" s="23" t="n">
+      <c r="S19" s="22" t="n">
         <f aca="false">R19/1000</f>
         <v>0.030204145</v>
       </c>
@@ -5340,25 +5106,25 @@
         <v>0</v>
       </c>
       <c r="E20" s="8"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="J20" s="31" t="n">
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="J20" s="29" t="n">
         <v>18.563083</v>
       </c>
-      <c r="K20" s="31" t="n">
+      <c r="K20" s="29" t="n">
         <v>12.257357</v>
       </c>
-      <c r="L20" s="31" t="n">
+      <c r="L20" s="29" t="n">
         <v>-2.859786</v>
       </c>
-      <c r="M20" s="31" t="n">
+      <c r="M20" s="29" t="n">
         <v>0.268238</v>
       </c>
-      <c r="N20" s="31" t="n">
+      <c r="N20" s="29" t="n">
         <v>1.97799</v>
       </c>
-      <c r="O20" s="31" t="n">
+      <c r="O20" s="29" t="n">
         <v>-1.147438</v>
       </c>
       <c r="P20" s="5" t="n">
@@ -5367,11 +5133,11 @@
       <c r="Q20" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="R20" s="22" t="n">
+      <c r="R20" s="16" t="n">
         <f aca="false">J20 + K20*Ti/1000 + L20*(Ti/1000)^2 + M20*(Ti/1000)^3 + N20/((Ti/1000)^2)</f>
         <v>30.206882</v>
       </c>
-      <c r="S20" s="23" t="n">
+      <c r="S20" s="22" t="n">
         <f aca="false">R20/1000</f>
         <v>0.030206882</v>
       </c>
@@ -5384,31 +5150,31 @@
         <v>2</v>
       </c>
       <c r="C21" s="8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="8" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="8"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="J21" s="31" t="n">
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="J21" s="29" t="n">
         <v>43.41356</v>
       </c>
-      <c r="K21" s="31" t="n">
+      <c r="K21" s="29" t="n">
         <v>-4.293079</v>
       </c>
-      <c r="L21" s="31" t="n">
+      <c r="L21" s="29" t="n">
         <v>1.272428</v>
       </c>
-      <c r="M21" s="31" t="n">
+      <c r="M21" s="29" t="n">
         <v>-0.096876</v>
       </c>
-      <c r="N21" s="31" t="n">
+      <c r="N21" s="29" t="n">
         <v>-20.533862</v>
       </c>
-      <c r="O21" s="31" t="n">
+      <c r="O21" s="29" t="n">
         <v>-38.515158</v>
       </c>
       <c r="P21" s="0" t="n">
@@ -5417,11 +5183,11 @@
       <c r="Q21" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="R21" s="22" t="n">
+      <c r="R21" s="16" t="n">
         <f aca="false">J21 + K21*Ti/1000 + L21*(Ti/1000)^2 + M21*(Ti/1000)^3 + N21/((Ti/1000)^2)</f>
         <v>19.762171</v>
       </c>
-      <c r="S21" s="23" t="n">
+      <c r="S21" s="22" t="n">
         <f aca="false">R21/1000</f>
         <v>0.019762171</v>
       </c>
@@ -5434,15 +5200,15 @@
         <v>1</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
     </row>
     <row r="23" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D23" s="8"/>
@@ -5453,15 +5219,18 @@
       <c r="G23" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="P23" s="34"/>
+      <c r="J23" s="31" t="n">
+        <f aca="false">J21*C7+K21*C7^2/2+L21*C7^3/3+M21*C7^4/4-N21/C7+O21</f>
+        <v>88.7414001666667</v>
+      </c>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+      <c r="P23" s="32"/>
     </row>
     <row r="24" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="8"/>
-      <c r="E24" s="35" t="s">
+      <c r="E24" s="33" t="s">
         <v>56</v>
       </c>
       <c r="F24" s="8" t="n">
@@ -5469,13 +5238,13 @@
         <v>-241.83</v>
       </c>
       <c r="G24" s="8" t="n">
-        <f aca="false">C22*F24</f>
+        <f aca="false">D21*F24</f>
         <v>-241.83</v>
       </c>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
     </row>
     <row r="25" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="13" t="s">
@@ -5488,7 +5257,7 @@
       <c r="E25" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="36" t="n">
+      <c r="F25" s="34" t="n">
         <f aca="false">J8*Tfuel/1000 + K8*((Tfuel/1000)^2)/2 + L8*(Tfuel/1000)^3/3 + M8*(Tfuel/1000)^4/4  - N8/(Tfuel/1000) + O8 - P8</f>
         <v>0.0672044823666624</v>
       </c>
@@ -5496,13 +5265,13 @@
         <f aca="false">-C17*F25</f>
         <v>-0</v>
       </c>
-      <c r="J25" s="33"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
     </row>
     <row r="26" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="35" t="s">
         <v>56</v>
       </c>
       <c r="B26" s="8" t="n">
@@ -5516,21 +5285,21 @@
       <c r="E26" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F26" s="36" t="n">
+      <c r="F26" s="34" t="n">
         <f aca="false">IF(Toxid&lt;700, J9*Toxid/1000 + K9*((Toxid/1000)^2)/2 + L9*(Toxid/1000)^3/3 + M9*(Toxid/1000)^4/4  - N9/(Toxid/1000) + O9 - P9, IF(Toxid&lt;2000, J10*Toxid/1000 + K10*((Toxid/1000)^2)/2 + L10*(Toxid/1000)^3/3 + M10*(Toxid/1000)^4/4  - N10/(Toxid/1000) + O10 - P10, J11*Toxid/1000 + K11*((Toxid/1000)^2)/2 + L11*(Toxid/1000)^3/3 + M11*(Toxid/1000)^4/4  - N11/(Toxid/1000) + O11 - P11))</f>
         <v>0.0539933240000021</v>
       </c>
       <c r="G26" s="17" t="n">
         <f aca="false">-C18*F26</f>
-        <v>-0.0269966620000011</v>
-      </c>
-      <c r="J26" s="33"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
+        <v>-0</v>
+      </c>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
     </row>
     <row r="27" customFormat="false" ht="17.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B27" s="8" t="n">
@@ -5543,21 +5312,21 @@
       <c r="E27" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F27" s="36" t="n">
+      <c r="F27" s="34" t="n">
         <f aca="false">IF(Toxid&lt;1000, J19*Toxid/1000 + K19*((Toxid/1000)^2)/2 + L19*(Toxid/1000)^3/3 + M19*(Toxid/1000)^4/4  - N19/(Toxid/1000) + O19 - P19, IF(Toxid&lt;2500, J20*Toxid/1000 + K20*((Toxid/1000)^2)/2 + L20*(Toxid/1000)^3/3 + M20*(Toxid/1000)^4/4  - N20/(Toxid/1000) + O20 - P20, J21*Toxid/1000 + K21*((Toxid/1000)^2)/2 + L21*(Toxid/1000)^3/3 + M21*(Toxid/1000)^4/4  - N21/(Toxid/1000) + O21 - P21))</f>
         <v>0.0535095758166655</v>
       </c>
       <c r="G27" s="17" t="n">
         <f aca="false">-C22*F27</f>
-        <v>-0.0535095758166655</v>
-      </c>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
+        <v>-0</v>
+      </c>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
     </row>
     <row r="28" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="35" t="s">
         <v>63</v>
       </c>
       <c r="B28" s="8" t="n">
@@ -5570,21 +5339,21 @@
       <c r="E28" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="38" t="n">
+      <c r="F28" s="36" t="n">
         <f aca="false">IF(Tout&lt;700, J19*Tout/1000 + K9*((Tout/1000)^2)/2 + L9*(Tout/1000)^3/3 + M9*(Tout/1000)^4/4  - N9/(Tout/1000) + O9 - P9, IF(Tout&lt;2000, J20*Tout/1000 + K10*((Tout/1000)^2)/2 + L10*(Tout/1000)^3/3 + M10*(Tout/1000)^4/4  - N10/(Tout/1000) + O10 - P10, J21*Tout/1000 + K11*((Tout/1000)^2)/2 + L11*(Tout/1000)^3/3 + M11*(Tout/1000)^4/4  - N11/(Tout/1000) + O11 - P11))</f>
-        <v>286.189686609564</v>
+        <v>165.520728916667</v>
       </c>
       <c r="G28" s="17" t="n">
         <f aca="false">F28*D18</f>
         <v>0</v>
       </c>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
     </row>
     <row r="29" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="35" t="s">
         <v>65</v>
       </c>
       <c r="B29" s="8" t="n">
@@ -5596,21 +5365,21 @@
       <c r="E29" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F29" s="38" t="n">
+      <c r="F29" s="36" t="n">
         <f aca="false">IF(Tout&lt;500, J12*Tout/1000 + K12*((Tout/1000)^2)/2 + L12*(Tout/1000)^3/3 + M12*(Tout/1000)^4/4  - N12/(Tout/1000) + O12 - P12, IF(Tout&lt;2000, J13*Tout/1000 + K13*((Tout/1000)^2)/2 + L13*(Tout/1000)^3/3 + M13*(Tout/1000)^4/4  - N13/(Tout/1000) + O13 - P13, J14*Tout/1000 + K14*((Tout/1000)^2)/2 + L14*(Tout/1000)^3/3 + M14*(Tout/1000)^4/4  - N14/(Tout/1000) + O14 - P14))</f>
-        <v>163.646865673573</v>
+        <v>92.7142383333333</v>
       </c>
       <c r="G29" s="17" t="n">
         <f aca="false">F29*D19</f>
         <v>0</v>
       </c>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="33"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
     </row>
     <row r="30" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="35" t="s">
         <v>67</v>
       </c>
       <c r="B30" s="8" t="n">
@@ -5622,85 +5391,85 @@
       <c r="E30" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F30" s="38" t="n">
+      <c r="F30" s="36" t="n">
         <f aca="false">IF(Tout&lt;1200, J15*Tout/1000 + K15*((Tout/1000)^2)/2 + L15*(Tout/1000)^3/3 + M15*(Tout/1000)^4/4  - N15/(Tout/1000) + O15 - P15, J16*Tout/1000 + K16*((Tout/1000)^2)/2 + L16*(Tout/1000)^3/3 + M16*(Tout/1000)^4/4  - N16/(Tout/1000) + O16 - P16)</f>
-        <v>272.328231115351</v>
+        <v>152.846797666667</v>
       </c>
       <c r="G30" s="17" t="n">
         <f aca="false">F30*D20</f>
         <v>0</v>
       </c>
-      <c r="J30" s="33"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="33"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="31"/>
     </row>
     <row r="31" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="25" t="s">
         <v>69</v>
       </c>
       <c r="B31" s="8"/>
       <c r="E31" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="F31" s="39" t="n">
+      <c r="F31" s="37" t="n">
         <f aca="false">IF(Tout&lt;1700, J17*Tout/1000 + K17*((Tout/1000)^2)/2 + L17*(Tout/1000)^3/3 + M17*(Tout/1000)^4/4  - N17/(Tout/1000) + O17 - P17, J18*Tout/1000 + K18*((Tout/1000)^2)/2 + L18*(Tout/1000)^3/3 + M18*(Tout/1000)^4/4  - N18/(Tout/1000) + O18 - P18)</f>
-        <v>235.869109934556</v>
+        <v>126.545643333333</v>
       </c>
       <c r="G31" s="17" t="n">
         <f aca="false">F31*D21</f>
-        <v>235.869109934556</v>
-      </c>
-      <c r="J31" s="33"/>
-      <c r="K31" s="33"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="33"/>
+        <v>126.545643333333</v>
+      </c>
+      <c r="J31" s="31"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="31"/>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F32" s="40" t="s">
+      <c r="F32" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="G32" s="41" t="n">
+      <c r="G32" s="38" t="n">
         <f aca="false">SUM(G24:G31)</f>
-        <v>-6.04139630326085</v>
-      </c>
-      <c r="J32" s="33"/>
-      <c r="K32" s="33"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="33"/>
+        <v>-115.284356666667</v>
+      </c>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="31"/>
+      <c r="M33" s="31"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J34" s="33"/>
-      <c r="K34" s="33"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="33"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="31"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J35" s="33"/>
-      <c r="K35" s="33"/>
-      <c r="L35" s="33"/>
-      <c r="M35" s="33"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J36" s="33"/>
-      <c r="K36" s="33"/>
-      <c r="L36" s="33"/>
-      <c r="M36" s="33"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J37" s="33"/>
-      <c r="K37" s="33"/>
-      <c r="L37" s="33"/>
-      <c r="M37" s="33"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="31"/>
     </row>
     <row r="38" customFormat="false" ht="17.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5731,7 +5500,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.57"/>
@@ -5745,7 +5514,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="39" t="s">
         <v>74</v>
       </c>
       <c r="E2" s="13" t="s">
@@ -5760,10 +5529,10 @@
       <c r="J2" s="13"/>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="13" t="s">
         <v>78</v>
       </c>
       <c r="G3" s="13" t="s">
@@ -5780,16 +5549,16 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="46" t="n">
+      <c r="C4" s="42" t="n">
         <v>-2657</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="47" t="n">
+      <c r="E4" s="28" t="n">
         <v>5</v>
       </c>
       <c r="F4" s="8" t="s">
@@ -5798,28 +5567,28 @@
       <c r="G4" s="8" t="n">
         <v>29.163</v>
       </c>
-      <c r="H4" s="23" t="n">
+      <c r="H4" s="22" t="n">
         <v>0.01449</v>
       </c>
-      <c r="I4" s="32" t="n">
+      <c r="I4" s="30" t="n">
         <v>-2.02E-006</v>
       </c>
-      <c r="J4" s="32" t="n">
+      <c r="J4" s="30" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="49" t="n">
+      <c r="C5" s="44" t="n">
         <f aca="false">C4+K12</f>
         <v>-0.91459435541492</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="47" t="n">
+      <c r="E5" s="28" t="n">
         <v>6.5</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -5828,24 +5597,24 @@
       <c r="G5" s="8" t="n">
         <v>25.46</v>
       </c>
-      <c r="H5" s="23" t="n">
+      <c r="H5" s="22" t="n">
         <v>0.01519</v>
       </c>
-      <c r="I5" s="32" t="n">
+      <c r="I5" s="30" t="n">
         <v>-7.15E-006</v>
       </c>
-      <c r="J5" s="32" t="n">
+      <c r="J5" s="30" t="n">
         <v>1.311E-009</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="51" t="n">
+      <c r="C6" s="46" t="n">
         <v>1510</v>
       </c>
-      <c r="E6" s="47" t="n">
+      <c r="E6" s="28" t="n">
         <v>48.9</v>
       </c>
       <c r="F6" s="8" t="s">
@@ -5854,18 +5623,18 @@
       <c r="G6" s="8" t="n">
         <v>28.883</v>
       </c>
-      <c r="H6" s="23" t="n">
+      <c r="H6" s="22" t="n">
         <v>-0.00157</v>
       </c>
-      <c r="I6" s="32" t="n">
+      <c r="I6" s="30" t="n">
         <v>8.08E-006</v>
       </c>
-      <c r="J6" s="32" t="n">
+      <c r="J6" s="30" t="n">
         <v>-2.871E-009</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="47" t="n">
+      <c r="E7" s="28" t="n">
         <v>4</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -5874,37 +5643,37 @@
       <c r="G7" s="8" t="n">
         <v>22.243</v>
       </c>
-      <c r="H7" s="23" t="n">
+      <c r="H7" s="22" t="n">
         <v>0.05977</v>
       </c>
-      <c r="I7" s="32" t="n">
+      <c r="I7" s="30" t="n">
         <v>-3.499E-005</v>
       </c>
-      <c r="J7" s="32" t="n">
+      <c r="J7" s="30" t="n">
         <v>7.464E-009</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="H9" s="52" t="s">
+      <c r="H9" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="I9" s="52" t="s">
+      <c r="I9" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="J9" s="52" t="s">
+      <c r="J9" s="47" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F10" s="8"/>
-      <c r="G10" s="53" t="n">
+      <c r="G10" s="48" t="n">
         <f aca="false">nH2O*G4+nO2a*G5+nN2a*G6+nCO2a*G7</f>
         <v>1812.6557</v>
       </c>
-      <c r="H10" s="23" t="n">
+      <c r="H10" s="22" t="n">
         <f aca="false">nH2O*H4+nO2a*H5+nN2a*H6+nCO2a*H7</f>
         <v>0.333492</v>
       </c>
@@ -5937,11 +5706,11 @@
         <f aca="false">G10*(T-298)</f>
         <v>2196938.7084</v>
       </c>
-      <c r="H12" s="53" t="n">
+      <c r="H12" s="48" t="n">
         <f aca="false">(H10/2)*(T^2-298^2)</f>
         <v>365389.842816</v>
       </c>
-      <c r="I12" s="53" t="n">
+      <c r="I12" s="48" t="n">
         <f aca="false">(I10/3)*(T^3-298^3)</f>
         <v>226145.273339472</v>
       </c>
@@ -5949,11 +5718,11 @@
         <f aca="false">(J10/4)*(T^4-298^4)</f>
         <v>-132388.418910887</v>
       </c>
-      <c r="K12" s="54" t="n">
+      <c r="K12" s="49" t="n">
         <f aca="false">SUM(G12:J12)/1000</f>
         <v>2656.08540564458</v>
       </c>
-      <c r="L12" s="55" t="s">
+      <c r="L12" s="50" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>